<commit_message>
added a lot of new information
</commit_message>
<xml_diff>
--- a/Lanphere_Arthropod_Morphospecies.xlsx
+++ b/Lanphere_Arthropod_Morphospecies.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="1400" yWindow="780" windowWidth="20120" windowHeight="13780" tabRatio="500"/>
+    <workbookView xWindow="1400" yWindow="780" windowWidth="20120" windowHeight="13780" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Nickname</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -70,6 +70,18 @@
   </si>
   <si>
     <t>Spider 1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Colladonus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>reductus</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Leafhopper brown/blue</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -438,10 +450,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" mc:Ignorable="mv" mc:PreserveAttributes="mv:*">
-  <dimension ref="A1:L2"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageLayout" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13"/>
@@ -497,6 +509,20 @@
         <v>12</v>
       </c>
     </row>
+    <row r="3" spans="1:12">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" t="s">
+        <v>14</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>